<commit_message>
update lookup table with correct values
</commit_message>
<xml_diff>
--- a/TemperatureConversionCalc/TemperatureConversion.xlsx
+++ b/TemperatureConversionCalc/TemperatureConversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdelkassara/Documents/University/3rd Year/2nd term/ECE 3375/ECE3375_Design_Project/TemperatureConversionCalc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE913C5B-CDC4-8F4A-A9B4-B80E898F7957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9011B32-2A51-F44C-8306-0A317E040D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{F4147E4D-230A-4444-B039-2B57AA445FAD}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{F4147E4D-230A-4444-B039-2B57AA445FAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>12bit temperature sensor value</t>
   </si>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>val adc</t>
-  </si>
-  <si>
-    <t>0000000</t>
-  </si>
-  <si>
-    <t>this is hard coded it's not really accurate</t>
   </si>
 </sst>
 </file>
@@ -464,7 +458,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,20 +530,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E3B8B9-5844-F24E-B6E7-BE393B772C84}">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
     <col min="2" max="2" width="33.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -562,11 +557,11 @@
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-25</v>
       </c>
@@ -575,18 +570,22 @@
         <v>FFFFFFE7</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.CONCAT($G$2,B2)</f>
+        <f>_xlfn.CONCAT($I$2,B2)</f>
         <v>.word 0xFFFFFFE7</v>
       </c>
       <c r="D2" t="str">
         <f>DEC2HEX((A2+25)*(2^5 -1),3)</f>
         <v>000</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2">
+        <f>HEX2DEC(D2)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-24</v>
       </c>
@@ -595,18 +594,20 @@
         <v>FFFFFFE8</v>
       </c>
       <c r="C3" t="str">
-        <f>_xlfn.CONCAT($G$2,B3)</f>
+        <f>_xlfn.CONCAT($I$2,B3)</f>
         <v>.word 0xFFFFFFE8</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D66" si="1">DEC2HEX((A3+25)*(2^5),3)</f>
         <v>020</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="2">HEX2DEC(D3)</f>
+        <v>32</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-23</v>
       </c>
@@ -615,15 +616,19 @@
         <v>FFFFFFE9</v>
       </c>
       <c r="C4" t="str">
-        <f>_xlfn.CONCAT($G$2,B4)</f>
+        <f>_xlfn.CONCAT($I$2,B4)</f>
         <v>.word 0xFFFFFFE9</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
         <v>040</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-22</v>
       </c>
@@ -632,15 +637,19 @@
         <v>FFFFFFEA</v>
       </c>
       <c r="C5" t="str">
-        <f>_xlfn.CONCAT($G$2,B5)</f>
+        <f>_xlfn.CONCAT($I$2,B5)</f>
         <v>.word 0xFFFFFFEA</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
         <v>060</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-21</v>
       </c>
@@ -649,15 +658,19 @@
         <v>FFFFFFEB</v>
       </c>
       <c r="C6" t="str">
-        <f>_xlfn.CONCAT($G$2,B6)</f>
+        <f>_xlfn.CONCAT($I$2,B6)</f>
         <v>.word 0xFFFFFFEB</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
         <v>080</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-20</v>
       </c>
@@ -666,15 +679,19 @@
         <v>FFFFFFEC</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT($G$2,B7)</f>
+        <f>_xlfn.CONCAT($I$2,B7)</f>
         <v>.word 0xFFFFFFEC</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>0A0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-19</v>
       </c>
@@ -683,15 +700,19 @@
         <v>FFFFFFED</v>
       </c>
       <c r="C8" t="str">
-        <f>_xlfn.CONCAT($G$2,B8)</f>
+        <f>_xlfn.CONCAT($I$2,B8)</f>
         <v>.word 0xFFFFFFED</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
         <v>0C0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-18</v>
       </c>
@@ -700,15 +721,19 @@
         <v>FFFFFFEE</v>
       </c>
       <c r="C9" t="str">
-        <f>_xlfn.CONCAT($G$2,B9)</f>
+        <f>_xlfn.CONCAT($I$2,B9)</f>
         <v>.word 0xFFFFFFEE</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
         <v>0E0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-17</v>
       </c>
@@ -717,15 +742,19 @@
         <v>FFFFFFEF</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT($G$2,B10)</f>
+        <f>_xlfn.CONCAT($I$2,B10)</f>
         <v>.word 0xFFFFFFEF</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-16</v>
       </c>
@@ -734,15 +763,19 @@
         <v>FFFFFFF0</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.CONCAT($G$2,B11)</f>
+        <f>_xlfn.CONCAT($I$2,B11)</f>
         <v>.word 0xFFFFFFF0</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-15</v>
       </c>
@@ -751,15 +784,19 @@
         <v>FFFFFFF1</v>
       </c>
       <c r="C12" t="str">
-        <f>_xlfn.CONCAT($G$2,B12)</f>
+        <f>_xlfn.CONCAT($I$2,B12)</f>
         <v>.word 0xFFFFFFF1</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-14</v>
       </c>
@@ -768,15 +805,19 @@
         <v>FFFFFFF2</v>
       </c>
       <c r="C13" t="str">
-        <f>_xlfn.CONCAT($G$2,B13)</f>
+        <f>_xlfn.CONCAT($I$2,B13)</f>
         <v>.word 0xFFFFFFF2</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-13</v>
       </c>
@@ -785,15 +826,19 @@
         <v>FFFFFFF3</v>
       </c>
       <c r="C14" t="str">
-        <f>_xlfn.CONCAT($G$2,B14)</f>
+        <f>_xlfn.CONCAT($I$2,B14)</f>
         <v>.word 0xFFFFFFF3</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-12</v>
       </c>
@@ -802,15 +847,19 @@
         <v>FFFFFFF4</v>
       </c>
       <c r="C15" t="str">
-        <f>_xlfn.CONCAT($G$2,B15)</f>
+        <f>_xlfn.CONCAT($I$2,B15)</f>
         <v>.word 0xFFFFFFF4</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
         <v>1A0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-11</v>
       </c>
@@ -819,15 +868,19 @@
         <v>FFFFFFF5</v>
       </c>
       <c r="C16" t="str">
-        <f>_xlfn.CONCAT($G$2,B16)</f>
+        <f>_xlfn.CONCAT($I$2,B16)</f>
         <v>.word 0xFFFFFFF5</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
         <v>1C0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-10</v>
       </c>
@@ -836,15 +889,19 @@
         <v>FFFFFFF6</v>
       </c>
       <c r="C17" t="str">
-        <f>_xlfn.CONCAT($G$2,B17)</f>
+        <f>_xlfn.CONCAT($I$2,B17)</f>
         <v>.word 0xFFFFFFF6</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
         <v>1E0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-9</v>
       </c>
@@ -853,15 +910,19 @@
         <v>FFFFFFF7</v>
       </c>
       <c r="C18" t="str">
-        <f>_xlfn.CONCAT($G$2,B18)</f>
+        <f>_xlfn.CONCAT($I$2,B18)</f>
         <v>.word 0xFFFFFFF7</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-8</v>
       </c>
@@ -870,15 +931,19 @@
         <v>FFFFFFF8</v>
       </c>
       <c r="C19" t="str">
-        <f>_xlfn.CONCAT($G$2,B19)</f>
+        <f>_xlfn.CONCAT($I$2,B19)</f>
         <v>.word 0xFFFFFFF8</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-7</v>
       </c>
@@ -887,15 +952,19 @@
         <v>FFFFFFF9</v>
       </c>
       <c r="C20" t="str">
-        <f>_xlfn.CONCAT($G$2,B20)</f>
+        <f>_xlfn.CONCAT($I$2,B20)</f>
         <v>.word 0xFFFFFFF9</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-6</v>
       </c>
@@ -904,15 +973,19 @@
         <v>FFFFFFFA</v>
       </c>
       <c r="C21" t="str">
-        <f>_xlfn.CONCAT($G$2,B21)</f>
+        <f>_xlfn.CONCAT($I$2,B21)</f>
         <v>.word 0xFFFFFFFA</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
         <v>260</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>608</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-5</v>
       </c>
@@ -921,15 +994,19 @@
         <v>FFFFFFFB</v>
       </c>
       <c r="C22" t="str">
-        <f>_xlfn.CONCAT($G$2,B22)</f>
+        <f>_xlfn.CONCAT($I$2,B22)</f>
         <v>.word 0xFFFFFFFB</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-4</v>
       </c>
@@ -938,15 +1015,19 @@
         <v>FFFFFFFC</v>
       </c>
       <c r="C23" t="str">
-        <f>_xlfn.CONCAT($G$2,B23)</f>
+        <f>_xlfn.CONCAT($I$2,B23)</f>
         <v>.word 0xFFFFFFFC</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
         <v>2A0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>672</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-3</v>
       </c>
@@ -955,15 +1036,19 @@
         <v>FFFFFFFD</v>
       </c>
       <c r="C24" t="str">
-        <f>_xlfn.CONCAT($G$2,B24)</f>
+        <f>_xlfn.CONCAT($I$2,B24)</f>
         <v>.word 0xFFFFFFFD</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
         <v>2C0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>704</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-2</v>
       </c>
@@ -972,15 +1057,19 @@
         <v>FFFFFFFE</v>
       </c>
       <c r="C25" t="str">
-        <f>_xlfn.CONCAT($G$2,B25)</f>
+        <f>_xlfn.CONCAT($I$2,B25)</f>
         <v>.word 0xFFFFFFFE</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
         <v>2E0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>736</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-1</v>
       </c>
@@ -989,15 +1078,19 @@
         <v>FFFFFFFF</v>
       </c>
       <c r="C26" t="str">
-        <f>_xlfn.CONCAT($G$2,B26)</f>
+        <f>_xlfn.CONCAT($I$2,B26)</f>
         <v>.word 0xFFFFFFFF</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1006,15 +1099,19 @@
         <v>00000000</v>
       </c>
       <c r="C27" t="str">
-        <f>_xlfn.CONCAT($G$2,B27)</f>
+        <f>_xlfn.CONCAT($I$2,B27)</f>
         <v>.word 0x00000000</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
         <v>320</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1023,15 +1120,19 @@
         <v>00000001</v>
       </c>
       <c r="C28" t="str">
-        <f>_xlfn.CONCAT($G$2,B28)</f>
+        <f>_xlfn.CONCAT($I$2,B28)</f>
         <v>.word 0x00000001</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>832</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1040,15 +1141,19 @@
         <v>00000002</v>
       </c>
       <c r="C29" t="str">
-        <f>_xlfn.CONCAT($G$2,B29)</f>
+        <f>_xlfn.CONCAT($I$2,B29)</f>
         <v>.word 0x00000002</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1057,15 +1162,19 @@
         <v>00000003</v>
       </c>
       <c r="C30" t="str">
-        <f>_xlfn.CONCAT($G$2,B30)</f>
+        <f>_xlfn.CONCAT($I$2,B30)</f>
         <v>.word 0x00000003</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
         <v>380</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1074,15 +1183,19 @@
         <v>00000004</v>
       </c>
       <c r="C31" t="str">
-        <f>_xlfn.CONCAT($G$2,B31)</f>
+        <f>_xlfn.CONCAT($I$2,B31)</f>
         <v>.word 0x00000004</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="1"/>
         <v>3A0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>928</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1091,15 +1204,19 @@
         <v>00000005</v>
       </c>
       <c r="C32" t="str">
-        <f>_xlfn.CONCAT($G$2,B32)</f>
+        <f>_xlfn.CONCAT($I$2,B32)</f>
         <v>.word 0x00000005</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="1"/>
         <v>3C0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1108,15 +1225,19 @@
         <v>00000006</v>
       </c>
       <c r="C33" t="str">
-        <f>_xlfn.CONCAT($G$2,B33)</f>
+        <f>_xlfn.CONCAT($I$2,B33)</f>
         <v>.word 0x00000006</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="1"/>
         <v>3E0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1125,15 +1246,19 @@
         <v>00000007</v>
       </c>
       <c r="C34" t="str">
-        <f>_xlfn.CONCAT($G$2,B34)</f>
+        <f>_xlfn.CONCAT($I$2,B34)</f>
         <v>.word 0x00000007</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1142,15 +1267,19 @@
         <v>00000008</v>
       </c>
       <c r="C35" t="str">
-        <f>_xlfn.CONCAT($G$2,B35)</f>
+        <f>_xlfn.CONCAT($I$2,B35)</f>
         <v>.word 0x00000008</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="1"/>
         <v>420</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>9</v>
       </c>
@@ -1159,15 +1288,19 @@
         <v>00000009</v>
       </c>
       <c r="C36" t="str">
-        <f>_xlfn.CONCAT($G$2,B36)</f>
+        <f>_xlfn.CONCAT($I$2,B36)</f>
         <v>.word 0x00000009</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="1"/>
         <v>440</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>10</v>
       </c>
@@ -1176,15 +1309,19 @@
         <v>0000000A</v>
       </c>
       <c r="C37" t="str">
-        <f>_xlfn.CONCAT($G$2,B37)</f>
+        <f>_xlfn.CONCAT($I$2,B37)</f>
         <v>.word 0x0000000A</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="1"/>
         <v>460</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>11</v>
       </c>
@@ -1193,15 +1330,19 @@
         <v>0000000B</v>
       </c>
       <c r="C38" t="str">
-        <f>_xlfn.CONCAT($G$2,B38)</f>
+        <f>_xlfn.CONCAT($I$2,B38)</f>
         <v>.word 0x0000000B</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>12</v>
       </c>
@@ -1210,15 +1351,19 @@
         <v>0000000C</v>
       </c>
       <c r="C39" t="str">
-        <f>_xlfn.CONCAT($G$2,B39)</f>
+        <f>_xlfn.CONCAT($I$2,B39)</f>
         <v>.word 0x0000000C</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
         <v>4A0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>13</v>
       </c>
@@ -1227,15 +1372,19 @@
         <v>0000000D</v>
       </c>
       <c r="C40" t="str">
-        <f>_xlfn.CONCAT($G$2,B40)</f>
+        <f>_xlfn.CONCAT($I$2,B40)</f>
         <v>.word 0x0000000D</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="1"/>
         <v>4C0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1244,15 +1393,19 @@
         <v>0000000E</v>
       </c>
       <c r="C41" t="str">
-        <f>_xlfn.CONCAT($G$2,B41)</f>
+        <f>_xlfn.CONCAT($I$2,B41)</f>
         <v>.word 0x0000000E</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
         <v>4E0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>15</v>
       </c>
@@ -1261,15 +1414,19 @@
         <v>0000000F</v>
       </c>
       <c r="C42" t="str">
-        <f>_xlfn.CONCAT($G$2,B42)</f>
+        <f>_xlfn.CONCAT($I$2,B42)</f>
         <v>.word 0x0000000F</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>16</v>
       </c>
@@ -1278,15 +1435,19 @@
         <v>00000010</v>
       </c>
       <c r="C43" t="str">
-        <f>_xlfn.CONCAT($G$2,B43)</f>
+        <f>_xlfn.CONCAT($I$2,B43)</f>
         <v>.word 0x00000010</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>17</v>
       </c>
@@ -1295,15 +1456,19 @@
         <v>00000011</v>
       </c>
       <c r="C44" t="str">
-        <f>_xlfn.CONCAT($G$2,B44)</f>
+        <f>_xlfn.CONCAT($I$2,B44)</f>
         <v>.word 0x00000011</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="1"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>18</v>
       </c>
@@ -1312,15 +1477,19 @@
         <v>00000012</v>
       </c>
       <c r="C45" t="str">
-        <f>_xlfn.CONCAT($G$2,B45)</f>
+        <f>_xlfn.CONCAT($I$2,B45)</f>
         <v>.word 0x00000012</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="1"/>
         <v>560</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>19</v>
       </c>
@@ -1329,15 +1498,19 @@
         <v>00000013</v>
       </c>
       <c r="C46" t="str">
-        <f>_xlfn.CONCAT($G$2,B46)</f>
+        <f>_xlfn.CONCAT($I$2,B46)</f>
         <v>.word 0x00000013</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
         <v>580</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20</v>
       </c>
@@ -1346,15 +1519,19 @@
         <v>00000014</v>
       </c>
       <c r="C47" t="str">
-        <f>_xlfn.CONCAT($G$2,B47)</f>
+        <f>_xlfn.CONCAT($I$2,B47)</f>
         <v>.word 0x00000014</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
         <v>5A0</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>21</v>
       </c>
@@ -1363,15 +1540,19 @@
         <v>00000015</v>
       </c>
       <c r="C48" t="str">
-        <f>_xlfn.CONCAT($G$2,B48)</f>
+        <f>_xlfn.CONCAT($I$2,B48)</f>
         <v>.word 0x00000015</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="1"/>
         <v>5C0</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>22</v>
       </c>
@@ -1380,15 +1561,19 @@
         <v>00000016</v>
       </c>
       <c r="C49" t="str">
-        <f>_xlfn.CONCAT($G$2,B49)</f>
+        <f>_xlfn.CONCAT($I$2,B49)</f>
         <v>.word 0x00000016</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
         <v>5E0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>23</v>
       </c>
@@ -1397,15 +1582,19 @@
         <v>00000017</v>
       </c>
       <c r="C50" t="str">
-        <f>_xlfn.CONCAT($G$2,B50)</f>
+        <f>_xlfn.CONCAT($I$2,B50)</f>
         <v>.word 0x00000017</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>24</v>
       </c>
@@ -1414,15 +1603,19 @@
         <v>00000018</v>
       </c>
       <c r="C51" t="str">
-        <f>_xlfn.CONCAT($G$2,B51)</f>
+        <f>_xlfn.CONCAT($I$2,B51)</f>
         <v>.word 0x00000018</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="1"/>
         <v>620</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>25</v>
       </c>
@@ -1431,15 +1624,19 @@
         <v>00000019</v>
       </c>
       <c r="C52" t="str">
-        <f>_xlfn.CONCAT($G$2,B52)</f>
+        <f>_xlfn.CONCAT($I$2,B52)</f>
         <v>.word 0x00000019</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="1"/>
         <v>640</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>26</v>
       </c>
@@ -1448,15 +1645,19 @@
         <v>0000001A</v>
       </c>
       <c r="C53" t="str">
-        <f>_xlfn.CONCAT($G$2,B53)</f>
+        <f>_xlfn.CONCAT($I$2,B53)</f>
         <v>.word 0x0000001A</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="1"/>
         <v>660</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>27</v>
       </c>
@@ -1465,15 +1666,19 @@
         <v>0000001B</v>
       </c>
       <c r="C54" t="str">
-        <f>_xlfn.CONCAT($G$2,B54)</f>
+        <f>_xlfn.CONCAT($I$2,B54)</f>
         <v>.word 0x0000001B</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="1"/>
         <v>680</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>28</v>
       </c>
@@ -1482,15 +1687,19 @@
         <v>0000001C</v>
       </c>
       <c r="C55" t="str">
-        <f>_xlfn.CONCAT($G$2,B55)</f>
+        <f>_xlfn.CONCAT($I$2,B55)</f>
         <v>.word 0x0000001C</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="1"/>
         <v>6A0</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>29</v>
       </c>
@@ -1499,15 +1708,19 @@
         <v>0000001D</v>
       </c>
       <c r="C56" t="str">
-        <f>_xlfn.CONCAT($G$2,B56)</f>
+        <f>_xlfn.CONCAT($I$2,B56)</f>
         <v>.word 0x0000001D</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="1"/>
         <v>6C0</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>30</v>
       </c>
@@ -1516,15 +1729,19 @@
         <v>0000001E</v>
       </c>
       <c r="C57" t="str">
-        <f>_xlfn.CONCAT($G$2,B57)</f>
+        <f>_xlfn.CONCAT($I$2,B57)</f>
         <v>.word 0x0000001E</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="1"/>
         <v>6E0</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>31</v>
       </c>
@@ -1533,15 +1750,19 @@
         <v>0000001F</v>
       </c>
       <c r="C58" t="str">
-        <f>_xlfn.CONCAT($G$2,B58)</f>
+        <f>_xlfn.CONCAT($I$2,B58)</f>
         <v>.word 0x0000001F</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>32</v>
       </c>
@@ -1550,15 +1771,19 @@
         <v>00000020</v>
       </c>
       <c r="C59" t="str">
-        <f>_xlfn.CONCAT($G$2,B59)</f>
+        <f>_xlfn.CONCAT($I$2,B59)</f>
         <v>.word 0x00000020</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>33</v>
       </c>
@@ -1567,15 +1792,19 @@
         <v>00000021</v>
       </c>
       <c r="C60" t="str">
-        <f>_xlfn.CONCAT($G$2,B60)</f>
+        <f>_xlfn.CONCAT($I$2,B60)</f>
         <v>.word 0x00000021</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="1"/>
         <v>740</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>34</v>
       </c>
@@ -1584,15 +1813,19 @@
         <v>00000022</v>
       </c>
       <c r="C61" t="str">
-        <f>_xlfn.CONCAT($G$2,B61)</f>
+        <f>_xlfn.CONCAT($I$2,B61)</f>
         <v>.word 0x00000022</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="1"/>
         <v>760</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>35</v>
       </c>
@@ -1601,15 +1834,19 @@
         <v>00000023</v>
       </c>
       <c r="C62" t="str">
-        <f>_xlfn.CONCAT($G$2,B62)</f>
+        <f>_xlfn.CONCAT($I$2,B62)</f>
         <v>.word 0x00000023</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="1"/>
         <v>780</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>36</v>
       </c>
@@ -1618,15 +1855,19 @@
         <v>00000024</v>
       </c>
       <c r="C63" t="str">
-        <f>_xlfn.CONCAT($G$2,B63)</f>
+        <f>_xlfn.CONCAT($I$2,B63)</f>
         <v>.word 0x00000024</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="1"/>
         <v>7A0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>37</v>
       </c>
@@ -1635,15 +1876,19 @@
         <v>00000025</v>
       </c>
       <c r="C64" t="str">
-        <f>_xlfn.CONCAT($G$2,B64)</f>
+        <f>_xlfn.CONCAT($I$2,B64)</f>
         <v>.word 0x00000025</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="1"/>
         <v>7C0</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>38</v>
       </c>
@@ -1652,15 +1897,19 @@
         <v>00000026</v>
       </c>
       <c r="C65" t="str">
-        <f>_xlfn.CONCAT($G$2,B65)</f>
+        <f>_xlfn.CONCAT($I$2,B65)</f>
         <v>.word 0x00000026</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="1"/>
         <v>7E0</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>39</v>
       </c>
@@ -1669,1066 +1918,1318 @@
         <v>00000027</v>
       </c>
       <c r="C66" t="str">
-        <f>_xlfn.CONCAT($G$2,B66)</f>
+        <f>_xlfn.CONCAT($I$2,B66)</f>
         <v>.word 0x00000027</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>40</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B130" si="2">RIGHT(DEC2HEX(A67,8), 8)</f>
+        <f t="shared" ref="B67:B130" si="3">RIGHT(DEC2HEX(A67,8), 8)</f>
         <v>00000028</v>
       </c>
       <c r="C67" t="str">
-        <f>_xlfn.CONCAT($G$2,B67)</f>
+        <f>_xlfn.CONCAT($I$2,B67)</f>
         <v>.word 0x00000028</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D130" si="3">DEC2HEX((A67+25)*(2^5),3)</f>
+        <f t="shared" ref="D67:D130" si="4">DEC2HEX((A67+25)*(2^5),3)</f>
         <v>820</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <f t="shared" ref="E67:E130" si="5">HEX2DEC(D67)</f>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>41</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000029</v>
       </c>
       <c r="C68" t="str">
-        <f>_xlfn.CONCAT($G$2,B68)</f>
+        <f>_xlfn.CONCAT($I$2,B68)</f>
         <v>.word 0x00000029</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>840</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <f t="shared" si="5"/>
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>42</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000002A</v>
       </c>
       <c r="C69" t="str">
-        <f>_xlfn.CONCAT($G$2,B69)</f>
+        <f>_xlfn.CONCAT($I$2,B69)</f>
         <v>.word 0x0000002A</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>860</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <f t="shared" si="5"/>
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>43</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000002B</v>
       </c>
       <c r="C70" t="str">
-        <f>_xlfn.CONCAT($G$2,B70)</f>
+        <f>_xlfn.CONCAT($I$2,B70)</f>
         <v>.word 0x0000002B</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>880</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <f t="shared" si="5"/>
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>44</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000002C</v>
       </c>
       <c r="C71" t="str">
-        <f>_xlfn.CONCAT($G$2,B71)</f>
+        <f>_xlfn.CONCAT($I$2,B71)</f>
         <v>.word 0x0000002C</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8A0</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <f t="shared" si="5"/>
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>45</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000002D</v>
       </c>
       <c r="C72" t="str">
-        <f>_xlfn.CONCAT($G$2,B72)</f>
+        <f>_xlfn.CONCAT($I$2,B72)</f>
         <v>.word 0x0000002D</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8C0</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <f t="shared" si="5"/>
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>46</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000002E</v>
       </c>
       <c r="C73" t="str">
-        <f>_xlfn.CONCAT($G$2,B73)</f>
+        <f>_xlfn.CONCAT($I$2,B73)</f>
         <v>.word 0x0000002E</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8E0</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <f t="shared" si="5"/>
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>47</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000002F</v>
       </c>
       <c r="C74" t="str">
-        <f>_xlfn.CONCAT($G$2,B74)</f>
+        <f>_xlfn.CONCAT($I$2,B74)</f>
         <v>.word 0x0000002F</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <f t="shared" si="5"/>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>48</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000030</v>
       </c>
       <c r="C75" t="str">
-        <f>_xlfn.CONCAT($G$2,B75)</f>
+        <f>_xlfn.CONCAT($I$2,B75)</f>
         <v>.word 0x00000030</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>920</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <f t="shared" si="5"/>
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>49</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000031</v>
       </c>
       <c r="C76" t="str">
-        <f>_xlfn.CONCAT($G$2,B76)</f>
+        <f>_xlfn.CONCAT($I$2,B76)</f>
         <v>.word 0x00000031</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>940</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <f t="shared" si="5"/>
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>50</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000032</v>
       </c>
       <c r="C77" t="str">
-        <f>_xlfn.CONCAT($G$2,B77)</f>
+        <f>_xlfn.CONCAT($I$2,B77)</f>
         <v>.word 0x00000032</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>960</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <f t="shared" si="5"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>51</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000033</v>
       </c>
       <c r="C78" t="str">
-        <f>_xlfn.CONCAT($G$2,B78)</f>
+        <f>_xlfn.CONCAT($I$2,B78)</f>
         <v>.word 0x00000033</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>980</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <f t="shared" si="5"/>
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>52</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000034</v>
       </c>
       <c r="C79" t="str">
-        <f>_xlfn.CONCAT($G$2,B79)</f>
+        <f>_xlfn.CONCAT($I$2,B79)</f>
         <v>.word 0x00000034</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9A0</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <f t="shared" si="5"/>
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>53</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000035</v>
       </c>
       <c r="C80" t="str">
-        <f>_xlfn.CONCAT($G$2,B80)</f>
+        <f>_xlfn.CONCAT($I$2,B80)</f>
         <v>.word 0x00000035</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9C0</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <f t="shared" si="5"/>
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>54</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000036</v>
       </c>
       <c r="C81" t="str">
-        <f>_xlfn.CONCAT($G$2,B81)</f>
+        <f>_xlfn.CONCAT($I$2,B81)</f>
         <v>.word 0x00000036</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9E0</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <f t="shared" si="5"/>
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>55</v>
       </c>
       <c r="B82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000037</v>
       </c>
       <c r="C82" t="str">
-        <f>_xlfn.CONCAT($G$2,B82)</f>
+        <f>_xlfn.CONCAT($I$2,B82)</f>
         <v>.word 0x00000037</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>A00</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <f t="shared" si="5"/>
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>56</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000038</v>
       </c>
       <c r="C83" t="str">
-        <f>_xlfn.CONCAT($G$2,B83)</f>
+        <f>_xlfn.CONCAT($I$2,B83)</f>
         <v>.word 0x00000038</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>A20</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <f t="shared" si="5"/>
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>57</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000039</v>
       </c>
       <c r="C84" t="str">
-        <f>_xlfn.CONCAT($G$2,B84)</f>
+        <f>_xlfn.CONCAT($I$2,B84)</f>
         <v>.word 0x00000039</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>A40</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <f t="shared" si="5"/>
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>58</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000003A</v>
       </c>
       <c r="C85" t="str">
-        <f>_xlfn.CONCAT($G$2,B85)</f>
+        <f>_xlfn.CONCAT($I$2,B85)</f>
         <v>.word 0x0000003A</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>A60</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <f t="shared" si="5"/>
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>59</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000003B</v>
       </c>
       <c r="C86" t="str">
-        <f>_xlfn.CONCAT($G$2,B86)</f>
+        <f>_xlfn.CONCAT($I$2,B86)</f>
         <v>.word 0x0000003B</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>A80</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <f t="shared" si="5"/>
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>60</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000003C</v>
       </c>
       <c r="C87" t="str">
-        <f>_xlfn.CONCAT($G$2,B87)</f>
+        <f>_xlfn.CONCAT($I$2,B87)</f>
         <v>.word 0x0000003C</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>AA0</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <f t="shared" si="5"/>
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>61</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000003D</v>
       </c>
       <c r="C88" t="str">
-        <f>_xlfn.CONCAT($G$2,B88)</f>
+        <f>_xlfn.CONCAT($I$2,B88)</f>
         <v>.word 0x0000003D</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>AC0</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <f t="shared" si="5"/>
+        <v>2752</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>62</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000003E</v>
       </c>
       <c r="C89" t="str">
-        <f>_xlfn.CONCAT($G$2,B89)</f>
+        <f>_xlfn.CONCAT($I$2,B89)</f>
         <v>.word 0x0000003E</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>AE0</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <f t="shared" si="5"/>
+        <v>2784</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>63</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000003F</v>
       </c>
       <c r="C90" t="str">
-        <f>_xlfn.CONCAT($G$2,B90)</f>
+        <f>_xlfn.CONCAT($I$2,B90)</f>
         <v>.word 0x0000003F</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>B00</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <f t="shared" si="5"/>
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>64</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000040</v>
       </c>
       <c r="C91" t="str">
-        <f>_xlfn.CONCAT($G$2,B91)</f>
+        <f>_xlfn.CONCAT($I$2,B91)</f>
         <v>.word 0x00000040</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>B20</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <f t="shared" si="5"/>
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>65</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000041</v>
       </c>
       <c r="C92" t="str">
-        <f>_xlfn.CONCAT($G$2,B92)</f>
+        <f>_xlfn.CONCAT($I$2,B92)</f>
         <v>.word 0x00000041</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>B40</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <f t="shared" si="5"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>66</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000042</v>
       </c>
       <c r="C93" t="str">
-        <f>_xlfn.CONCAT($G$2,B93)</f>
+        <f>_xlfn.CONCAT($I$2,B93)</f>
         <v>.word 0x00000042</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>B60</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <f t="shared" si="5"/>
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>67</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000043</v>
       </c>
       <c r="C94" t="str">
-        <f>_xlfn.CONCAT($G$2,B94)</f>
+        <f>_xlfn.CONCAT($I$2,B94)</f>
         <v>.word 0x00000043</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>B80</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <f t="shared" si="5"/>
+        <v>2944</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>68</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000044</v>
       </c>
       <c r="C95" t="str">
-        <f>_xlfn.CONCAT($G$2,B95)</f>
+        <f>_xlfn.CONCAT($I$2,B95)</f>
         <v>.word 0x00000044</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>BA0</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <f t="shared" si="5"/>
+        <v>2976</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>69</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000045</v>
       </c>
       <c r="C96" t="str">
-        <f>_xlfn.CONCAT($G$2,B96)</f>
+        <f>_xlfn.CONCAT($I$2,B96)</f>
         <v>.word 0x00000045</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>BC0</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <f t="shared" si="5"/>
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>70</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000046</v>
       </c>
       <c r="C97" t="str">
-        <f>_xlfn.CONCAT($G$2,B97)</f>
+        <f>_xlfn.CONCAT($I$2,B97)</f>
         <v>.word 0x00000046</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>BE0</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <f t="shared" si="5"/>
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>71</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000047</v>
       </c>
       <c r="C98" t="str">
-        <f>_xlfn.CONCAT($G$2,B98)</f>
+        <f>_xlfn.CONCAT($I$2,B98)</f>
         <v>.word 0x00000047</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C00</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <f t="shared" si="5"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>72</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000048</v>
       </c>
       <c r="C99" t="str">
-        <f>_xlfn.CONCAT($G$2,B99)</f>
+        <f>_xlfn.CONCAT($I$2,B99)</f>
         <v>.word 0x00000048</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C20</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <f t="shared" si="5"/>
+        <v>3104</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>73</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000049</v>
       </c>
       <c r="C100" t="str">
-        <f>_xlfn.CONCAT($G$2,B100)</f>
+        <f>_xlfn.CONCAT($I$2,B100)</f>
         <v>.word 0x00000049</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C40</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <f t="shared" si="5"/>
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>74</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000004A</v>
       </c>
       <c r="C101" t="str">
-        <f>_xlfn.CONCAT($G$2,B101)</f>
+        <f>_xlfn.CONCAT($I$2,B101)</f>
         <v>.word 0x0000004A</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C60</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <f t="shared" si="5"/>
+        <v>3168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>75</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000004B</v>
       </c>
       <c r="C102" t="str">
-        <f>_xlfn.CONCAT($G$2,B102)</f>
+        <f>_xlfn.CONCAT($I$2,B102)</f>
         <v>.word 0x0000004B</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C80</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <f t="shared" si="5"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>76</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000004C</v>
       </c>
       <c r="C103" t="str">
-        <f>_xlfn.CONCAT($G$2,B103)</f>
+        <f>_xlfn.CONCAT($I$2,B103)</f>
         <v>.word 0x0000004C</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CA0</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <f t="shared" si="5"/>
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>77</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000004D</v>
       </c>
       <c r="C104" t="str">
-        <f>_xlfn.CONCAT($G$2,B104)</f>
+        <f>_xlfn.CONCAT($I$2,B104)</f>
         <v>.word 0x0000004D</v>
       </c>
       <c r="D104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CC0</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <f t="shared" si="5"/>
+        <v>3264</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>78</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000004E</v>
       </c>
       <c r="C105" t="str">
-        <f>_xlfn.CONCAT($G$2,B105)</f>
+        <f>_xlfn.CONCAT($I$2,B105)</f>
         <v>.word 0x0000004E</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CE0</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <f t="shared" si="5"/>
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>79</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000004F</v>
       </c>
       <c r="C106" t="str">
-        <f>_xlfn.CONCAT($G$2,B106)</f>
+        <f>_xlfn.CONCAT($I$2,B106)</f>
         <v>.word 0x0000004F</v>
       </c>
       <c r="D106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D00</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <f t="shared" si="5"/>
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>80</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000050</v>
       </c>
       <c r="C107" t="str">
-        <f>_xlfn.CONCAT($G$2,B107)</f>
+        <f>_xlfn.CONCAT($I$2,B107)</f>
         <v>.word 0x00000050</v>
       </c>
       <c r="D107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D20</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <f t="shared" si="5"/>
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>81</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000051</v>
       </c>
       <c r="C108" t="str">
-        <f>_xlfn.CONCAT($G$2,B108)</f>
+        <f>_xlfn.CONCAT($I$2,B108)</f>
         <v>.word 0x00000051</v>
       </c>
       <c r="D108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D40</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <f t="shared" si="5"/>
+        <v>3392</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>82</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000052</v>
       </c>
       <c r="C109" t="str">
-        <f>_xlfn.CONCAT($G$2,B109)</f>
+        <f>_xlfn.CONCAT($I$2,B109)</f>
         <v>.word 0x00000052</v>
       </c>
       <c r="D109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D60</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <f t="shared" si="5"/>
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>83</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000053</v>
       </c>
       <c r="C110" t="str">
-        <f>_xlfn.CONCAT($G$2,B110)</f>
+        <f>_xlfn.CONCAT($I$2,B110)</f>
         <v>.word 0x00000053</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D80</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <f t="shared" si="5"/>
+        <v>3456</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>84</v>
       </c>
       <c r="B111" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000054</v>
       </c>
       <c r="C111" t="str">
-        <f>_xlfn.CONCAT($G$2,B111)</f>
+        <f>_xlfn.CONCAT($I$2,B111)</f>
         <v>.word 0x00000054</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DA0</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <f t="shared" si="5"/>
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>85</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000055</v>
       </c>
       <c r="C112" t="str">
-        <f>_xlfn.CONCAT($G$2,B112)</f>
+        <f>_xlfn.CONCAT($I$2,B112)</f>
         <v>.word 0x00000055</v>
       </c>
       <c r="D112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DC0</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <f t="shared" si="5"/>
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>86</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000056</v>
       </c>
       <c r="C113" t="str">
-        <f>_xlfn.CONCAT($G$2,B113)</f>
+        <f>_xlfn.CONCAT($I$2,B113)</f>
         <v>.word 0x00000056</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DE0</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <f t="shared" si="5"/>
+        <v>3552</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>87</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000057</v>
       </c>
       <c r="C114" t="str">
-        <f>_xlfn.CONCAT($G$2,B114)</f>
+        <f>_xlfn.CONCAT($I$2,B114)</f>
         <v>.word 0x00000057</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E00</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <f t="shared" si="5"/>
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>88</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000058</v>
       </c>
       <c r="C115" t="str">
-        <f>_xlfn.CONCAT($G$2,B115)</f>
+        <f>_xlfn.CONCAT($I$2,B115)</f>
         <v>.word 0x00000058</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E20</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <f t="shared" si="5"/>
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>89</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000059</v>
       </c>
       <c r="C116" t="str">
-        <f>_xlfn.CONCAT($G$2,B116)</f>
+        <f>_xlfn.CONCAT($I$2,B116)</f>
         <v>.word 0x00000059</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E40</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <f t="shared" si="5"/>
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>90</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000005A</v>
       </c>
       <c r="C117" t="str">
-        <f>_xlfn.CONCAT($G$2,B117)</f>
+        <f>_xlfn.CONCAT($I$2,B117)</f>
         <v>.word 0x0000005A</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E60</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <f t="shared" si="5"/>
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>91</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000005B</v>
       </c>
       <c r="C118" t="str">
-        <f>_xlfn.CONCAT($G$2,B118)</f>
+        <f>_xlfn.CONCAT($I$2,B118)</f>
         <v>.word 0x0000005B</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E80</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <f t="shared" si="5"/>
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>92</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000005C</v>
       </c>
       <c r="C119" t="str">
-        <f>_xlfn.CONCAT($G$2,B119)</f>
+        <f>_xlfn.CONCAT($I$2,B119)</f>
         <v>.word 0x0000005C</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>EA0</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <f t="shared" si="5"/>
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>93</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000005D</v>
       </c>
       <c r="C120" t="str">
-        <f>_xlfn.CONCAT($G$2,B120)</f>
+        <f>_xlfn.CONCAT($I$2,B120)</f>
         <v>.word 0x0000005D</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>EC0</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <f t="shared" si="5"/>
+        <v>3776</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>94</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000005E</v>
       </c>
       <c r="C121" t="str">
-        <f>_xlfn.CONCAT($G$2,B121)</f>
+        <f>_xlfn.CONCAT($I$2,B121)</f>
         <v>.word 0x0000005E</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>EE0</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <f t="shared" si="5"/>
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>95</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0000005F</v>
       </c>
       <c r="C122" t="str">
-        <f>_xlfn.CONCAT($G$2,B122)</f>
+        <f>_xlfn.CONCAT($I$2,B122)</f>
         <v>.word 0x0000005F</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F00</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E122">
+        <f t="shared" si="5"/>
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>96</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000060</v>
       </c>
       <c r="C123" t="str">
-        <f>_xlfn.CONCAT($G$2,B123)</f>
+        <f>_xlfn.CONCAT($I$2,B123)</f>
         <v>.word 0x00000060</v>
       </c>
       <c r="D123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F20</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <f t="shared" si="5"/>
+        <v>3872</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>97</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000061</v>
       </c>
       <c r="C124" t="str">
-        <f>_xlfn.CONCAT($G$2,B124)</f>
+        <f>_xlfn.CONCAT($I$2,B124)</f>
         <v>.word 0x00000061</v>
       </c>
       <c r="D124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F40</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E124">
+        <f t="shared" si="5"/>
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>98</v>
       </c>
       <c r="B125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000062</v>
       </c>
       <c r="C125" t="str">
-        <f>_xlfn.CONCAT($G$2,B125)</f>
+        <f>_xlfn.CONCAT($I$2,B125)</f>
         <v>.word 0x00000062</v>
       </c>
       <c r="D125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F60</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E125">
+        <f t="shared" si="5"/>
+        <v>3936</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>99</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000063</v>
       </c>
       <c r="C126" t="str">
-        <f>_xlfn.CONCAT($G$2,B126)</f>
+        <f>_xlfn.CONCAT($I$2,B126)</f>
         <v>.word 0x00000063</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F80</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E126">
+        <f t="shared" si="5"/>
+        <v>3968</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>100</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000064</v>
       </c>
       <c r="C127" t="str">
-        <f>_xlfn.CONCAT($G$2,B127)</f>
+        <f>_xlfn.CONCAT($I$2,B127)</f>
         <v>.word 0x00000064</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>FA0</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E127">
+        <f t="shared" si="5"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>101</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000065</v>
       </c>
       <c r="C128" t="str">
-        <f>_xlfn.CONCAT($G$2,B128)</f>
+        <f>_xlfn.CONCAT($I$2,B128)</f>
         <v>.word 0x00000065</v>
       </c>
       <c r="D128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>FC0</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="5"/>
+        <v>4032</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -2736,16 +3237,20 @@
         <v>102</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000066</v>
       </c>
       <c r="C129" t="str">
-        <f>_xlfn.CONCAT($G$2,B129)</f>
+        <f>_xlfn.CONCAT($I$2,B129)</f>
         <v>.word 0x00000066</v>
       </c>
       <c r="D129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>FE0</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="5"/>
+        <v>4064</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -2753,19 +3258,20 @@
         <v>103</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>00000067</v>
       </c>
       <c r="C130" t="str">
-        <f>_xlfn.CONCAT($G$2,B130)</f>
+        <f>_xlfn.CONCAT($I$2,B130)</f>
         <v>.word 0x00000067</v>
       </c>
       <c r="D130" t="str">
         <f>DEC2HEX((A130+25)*(2^5)-1,3)</f>
         <v>FFF</v>
       </c>
-      <c r="E130" t="s">
-        <v>16</v>
+      <c r="E130">
+        <f t="shared" si="5"/>
+        <v>4095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove unused file and add notes for what we have done
</commit_message>
<xml_diff>
--- a/TemperatureConversionCalc/TemperatureConversion.xlsx
+++ b/TemperatureConversionCalc/TemperatureConversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdelkassara/Documents/University/3rd Year/2nd term/ECE 3375/ECE3375_Design_Project/TemperatureConversionCalc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9011B32-2A51-F44C-8306-0A317E040D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178D3320-2A5B-944E-A8B8-0009FF01CE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{F4147E4D-230A-4444-B039-2B57AA445FAD}"/>
   </bookViews>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E3B8B9-5844-F24E-B6E7-BE393B772C84}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,6 +581,10 @@
         <f>HEX2DEC(D2)</f>
         <v>0</v>
       </c>
+      <c r="F2">
+        <f>(E2/4095)*3.3</f>
+        <v>0</v>
+      </c>
       <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
@@ -605,6 +609,10 @@
         <f t="shared" ref="E3:E66" si="2">HEX2DEC(D3)</f>
         <v>32</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="3">(E3/4095)*3.3</f>
+        <v>2.5787545787545788E-2</v>
+      </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -627,6 +635,10 @@
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>5.1575091575091575E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -648,6 +660,10 @@
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>7.7362637362637363E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -669,6 +685,10 @@
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>0.10315018315018315</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -690,6 +710,10 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>0.12893772893772892</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -711,6 +735,10 @@
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>0.15472527472527473</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -732,6 +760,10 @@
         <f t="shared" si="2"/>
         <v>224</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>0.1805128205128205</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -753,6 +785,10 @@
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>0.2063003663003663</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -774,6 +810,10 @@
         <f t="shared" si="2"/>
         <v>288</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>0.23208791208791207</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -795,6 +835,10 @@
         <f t="shared" si="2"/>
         <v>320</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>0.25787545787545785</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -816,6 +860,10 @@
         <f t="shared" si="2"/>
         <v>352</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>0.28366300366300362</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -837,6 +885,10 @@
         <f t="shared" si="2"/>
         <v>384</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>0.30945054945054945</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -858,6 +910,10 @@
         <f t="shared" si="2"/>
         <v>416</v>
       </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>0.33523809523809522</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -879,8 +935,12 @@
         <f t="shared" si="2"/>
         <v>448</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>0.361025641025641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-10</v>
       </c>
@@ -900,8 +960,12 @@
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>0.38681318681318677</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-9</v>
       </c>
@@ -921,8 +985,12 @@
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>0.4126007326007326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-8</v>
       </c>
@@ -942,8 +1010,12 @@
         <f t="shared" si="2"/>
         <v>544</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>0.43838827838827837</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-7</v>
       </c>
@@ -963,8 +1035,12 @@
         <f t="shared" si="2"/>
         <v>576</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>0.46417582417582415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-6</v>
       </c>
@@ -984,8 +1060,12 @@
         <f t="shared" si="2"/>
         <v>608</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>0.48996336996336992</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-5</v>
       </c>
@@ -1005,8 +1085,12 @@
         <f t="shared" si="2"/>
         <v>640</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>0.51575091575091569</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-4</v>
       </c>
@@ -1026,8 +1110,12 @@
         <f t="shared" si="2"/>
         <v>672</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>0.54153846153846152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-3</v>
       </c>
@@ -1047,8 +1135,12 @@
         <f t="shared" si="2"/>
         <v>704</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>0.56732600732600724</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-2</v>
       </c>
@@ -1068,8 +1160,12 @@
         <f t="shared" si="2"/>
         <v>736</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>0.59311355311355307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-1</v>
       </c>
@@ -1089,8 +1185,12 @@
         <f t="shared" si="2"/>
         <v>768</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>0.6189010989010989</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1110,8 +1210,12 @@
         <f t="shared" si="2"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>0.64468864468864462</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1131,8 +1235,12 @@
         <f t="shared" si="2"/>
         <v>832</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>0.67047619047619045</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1152,8 +1260,12 @@
         <f t="shared" si="2"/>
         <v>864</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>0.69626373626373628</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1173,8 +1285,12 @@
         <f t="shared" si="2"/>
         <v>896</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>0.722051282051282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1194,8 +1310,12 @@
         <f t="shared" si="2"/>
         <v>928</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>0.74783882783882782</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1215,8 +1335,12 @@
         <f t="shared" si="2"/>
         <v>960</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>0.77362637362637354</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1236,8 +1360,12 @@
         <f t="shared" si="2"/>
         <v>992</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>0.79941391941391937</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1257,8 +1385,12 @@
         <f t="shared" si="2"/>
         <v>1024</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <f t="shared" si="3"/>
+        <v>0.8252014652014652</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1278,8 +1410,12 @@
         <f t="shared" si="2"/>
         <v>1056</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>0.85098901098901103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>9</v>
       </c>
@@ -1299,8 +1435,12 @@
         <f t="shared" si="2"/>
         <v>1088</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>0.87677655677655675</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>10</v>
       </c>
@@ -1320,8 +1460,12 @@
         <f t="shared" si="2"/>
         <v>1120</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>0.90256410256410258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>11</v>
       </c>
@@ -1341,8 +1485,12 @@
         <f t="shared" si="2"/>
         <v>1152</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>0.9283516483516483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>12</v>
       </c>
@@ -1362,8 +1510,12 @@
         <f t="shared" si="2"/>
         <v>1184</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>0.95413919413919412</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>13</v>
       </c>
@@ -1383,8 +1535,12 @@
         <f t="shared" si="2"/>
         <v>1216</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>0.97992673992673984</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1404,8 +1560,12 @@
         <f t="shared" si="2"/>
         <v>1248</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <f t="shared" si="3"/>
+        <v>1.0057142857142858</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>15</v>
       </c>
@@ -1425,8 +1585,12 @@
         <f t="shared" si="2"/>
         <v>1280</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <f t="shared" si="3"/>
+        <v>1.0315018315018314</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>16</v>
       </c>
@@ -1446,8 +1610,12 @@
         <f t="shared" si="2"/>
         <v>1312</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <f t="shared" si="3"/>
+        <v>1.0572893772893772</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>17</v>
       </c>
@@ -1467,8 +1635,12 @@
         <f t="shared" si="2"/>
         <v>1344</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <f t="shared" si="3"/>
+        <v>1.083076923076923</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>18</v>
       </c>
@@ -1488,8 +1660,12 @@
         <f t="shared" si="2"/>
         <v>1376</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <f t="shared" si="3"/>
+        <v>1.1088644688644689</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>19</v>
       </c>
@@ -1509,8 +1685,12 @@
         <f t="shared" si="2"/>
         <v>1408</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <f t="shared" si="3"/>
+        <v>1.1346520146520145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20</v>
       </c>
@@ -1530,8 +1710,12 @@
         <f t="shared" si="2"/>
         <v>1440</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <f t="shared" si="3"/>
+        <v>1.1604395604395605</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>21</v>
       </c>
@@ -1551,8 +1735,12 @@
         <f t="shared" si="2"/>
         <v>1472</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>1.1862271062271061</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>22</v>
       </c>
@@ -1572,8 +1760,12 @@
         <f t="shared" si="2"/>
         <v>1504</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <f t="shared" si="3"/>
+        <v>1.212014652014652</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>23</v>
       </c>
@@ -1593,8 +1785,12 @@
         <f t="shared" si="2"/>
         <v>1536</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>1.2378021978021978</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>24</v>
       </c>
@@ -1614,8 +1810,12 @@
         <f t="shared" si="2"/>
         <v>1568</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>1.2635897435897436</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>25</v>
       </c>
@@ -1635,8 +1835,12 @@
         <f t="shared" si="2"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <f t="shared" si="3"/>
+        <v>1.2893772893772892</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>26</v>
       </c>
@@ -1656,8 +1860,12 @@
         <f t="shared" si="2"/>
         <v>1632</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <f t="shared" si="3"/>
+        <v>1.3151648351648353</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>27</v>
       </c>
@@ -1677,8 +1885,12 @@
         <f t="shared" si="2"/>
         <v>1664</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <f t="shared" si="3"/>
+        <v>1.3409523809523809</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>28</v>
       </c>
@@ -1698,8 +1910,12 @@
         <f t="shared" si="2"/>
         <v>1696</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <f t="shared" si="3"/>
+        <v>1.3667399267399267</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>29</v>
       </c>
@@ -1719,8 +1935,12 @@
         <f t="shared" si="2"/>
         <v>1728</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <f t="shared" si="3"/>
+        <v>1.3925274725274726</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>30</v>
       </c>
@@ -1740,8 +1960,12 @@
         <f t="shared" si="2"/>
         <v>1760</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <f t="shared" si="3"/>
+        <v>1.4183150183150184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>31</v>
       </c>
@@ -1761,8 +1985,12 @@
         <f t="shared" si="2"/>
         <v>1792</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <f t="shared" si="3"/>
+        <v>1.444102564102564</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>32</v>
       </c>
@@ -1782,8 +2010,12 @@
         <f t="shared" si="2"/>
         <v>1824</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <f t="shared" si="3"/>
+        <v>1.4698901098901098</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>33</v>
       </c>
@@ -1803,8 +2035,12 @@
         <f t="shared" si="2"/>
         <v>1856</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <f t="shared" si="3"/>
+        <v>1.4956776556776556</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>34</v>
       </c>
@@ -1824,8 +2060,12 @@
         <f t="shared" si="2"/>
         <v>1888</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <f t="shared" si="3"/>
+        <v>1.5214652014652015</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>35</v>
       </c>
@@ -1845,8 +2085,12 @@
         <f t="shared" si="2"/>
         <v>1920</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <f t="shared" si="3"/>
+        <v>1.5472527472527471</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>36</v>
       </c>
@@ -1866,8 +2110,12 @@
         <f t="shared" si="2"/>
         <v>1952</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <f t="shared" si="3"/>
+        <v>1.5730402930402931</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>37</v>
       </c>
@@ -1887,8 +2135,12 @@
         <f t="shared" si="2"/>
         <v>1984</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <f t="shared" si="3"/>
+        <v>1.5988278388278387</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>38</v>
       </c>
@@ -1908,8 +2160,12 @@
         <f t="shared" si="2"/>
         <v>2016</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <f t="shared" si="3"/>
+        <v>1.6246153846153846</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>39</v>
       </c>
@@ -1929,13 +2185,17 @@
         <f t="shared" si="2"/>
         <v>2048</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <f t="shared" si="3"/>
+        <v>1.6504029304029304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>40</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B130" si="3">RIGHT(DEC2HEX(A67,8), 8)</f>
+        <f t="shared" ref="B67:B130" si="4">RIGHT(DEC2HEX(A67,8), 8)</f>
         <v>00000028</v>
       </c>
       <c r="C67" t="str">
@@ -1943,20 +2203,24 @@
         <v>.word 0x00000028</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D130" si="4">DEC2HEX((A67+25)*(2^5),3)</f>
+        <f t="shared" ref="D67:D130" si="5">DEC2HEX((A67+25)*(2^5),3)</f>
         <v>820</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E130" si="5">HEX2DEC(D67)</f>
+        <f t="shared" ref="E67:E130" si="6">HEX2DEC(D67)</f>
         <v>2080</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="7">(E67/4095)*3.3</f>
+        <v>1.676190476190476</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>41</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000029</v>
       </c>
       <c r="C68" t="str">
@@ -1964,20 +2228,24 @@
         <v>.word 0x00000029</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>840</v>
       </c>
       <c r="E68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2112</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <f t="shared" si="7"/>
+        <v>1.7019780219780221</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>42</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000002A</v>
       </c>
       <c r="C69" t="str">
@@ -1985,20 +2253,24 @@
         <v>.word 0x0000002A</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>860</v>
       </c>
       <c r="E69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2144</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <f t="shared" si="7"/>
+        <v>1.7277655677655677</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>43</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000002B</v>
       </c>
       <c r="C70" t="str">
@@ -2006,20 +2278,24 @@
         <v>.word 0x0000002B</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>880</v>
       </c>
       <c r="E70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2176</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <f t="shared" si="7"/>
+        <v>1.7535531135531135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>44</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000002C</v>
       </c>
       <c r="C71" t="str">
@@ -2027,20 +2303,24 @@
         <v>.word 0x0000002C</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8A0</v>
       </c>
       <c r="E71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2208</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <f t="shared" si="7"/>
+        <v>1.7793406593406591</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>45</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000002D</v>
       </c>
       <c r="C72" t="str">
@@ -2048,20 +2328,24 @@
         <v>.word 0x0000002D</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8C0</v>
       </c>
       <c r="E72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2240</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <f t="shared" si="7"/>
+        <v>1.8051282051282052</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>46</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000002E</v>
       </c>
       <c r="C73" t="str">
@@ -2069,20 +2353,24 @@
         <v>.word 0x0000002E</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8E0</v>
       </c>
       <c r="E73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2272</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <f t="shared" si="7"/>
+        <v>1.830915750915751</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>47</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000002F</v>
       </c>
       <c r="C74" t="str">
@@ -2090,20 +2378,24 @@
         <v>.word 0x0000002F</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="E74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2304</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <f t="shared" si="7"/>
+        <v>1.8567032967032966</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>48</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000030</v>
       </c>
       <c r="C75" t="str">
@@ -2111,20 +2403,24 @@
         <v>.word 0x00000030</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>920</v>
       </c>
       <c r="E75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2336</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <f t="shared" si="7"/>
+        <v>1.8824908424908422</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>49</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000031</v>
       </c>
       <c r="C76" t="str">
@@ -2132,20 +2428,24 @@
         <v>.word 0x00000031</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>940</v>
       </c>
       <c r="E76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2368</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <f t="shared" si="7"/>
+        <v>1.9082783882783882</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>50</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000032</v>
       </c>
       <c r="C77" t="str">
@@ -2153,20 +2453,24 @@
         <v>.word 0x00000032</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>960</v>
       </c>
       <c r="E77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <f t="shared" si="7"/>
+        <v>1.9340659340659341</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>51</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000033</v>
       </c>
       <c r="C78" t="str">
@@ -2174,20 +2478,24 @@
         <v>.word 0x00000033</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>980</v>
       </c>
       <c r="E78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2432</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <f t="shared" si="7"/>
+        <v>1.9598534798534797</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>52</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000034</v>
       </c>
       <c r="C79" t="str">
@@ -2195,20 +2503,24 @@
         <v>.word 0x00000034</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9A0</v>
       </c>
       <c r="E79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2464</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <f t="shared" si="7"/>
+        <v>1.9856410256410255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>53</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000035</v>
       </c>
       <c r="C80" t="str">
@@ -2216,20 +2528,24 @@
         <v>.word 0x00000035</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9C0</v>
       </c>
       <c r="E80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2496</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <f t="shared" si="7"/>
+        <v>2.0114285714285716</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>54</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000036</v>
       </c>
       <c r="C81" t="str">
@@ -2237,20 +2553,24 @@
         <v>.word 0x00000036</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9E0</v>
       </c>
       <c r="E81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2528</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <f t="shared" si="7"/>
+        <v>2.0372161172161172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>55</v>
       </c>
       <c r="B82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000037</v>
       </c>
       <c r="C82" t="str">
@@ -2258,20 +2578,24 @@
         <v>.word 0x00000037</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>A00</v>
       </c>
       <c r="E82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2560</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <f t="shared" si="7"/>
+        <v>2.0630036630036628</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>56</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000038</v>
       </c>
       <c r="C83" t="str">
@@ -2279,20 +2603,24 @@
         <v>.word 0x00000038</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>A20</v>
       </c>
       <c r="E83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2592</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <f t="shared" si="7"/>
+        <v>2.0887912087912084</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>57</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000039</v>
       </c>
       <c r="C84" t="str">
@@ -2300,20 +2628,24 @@
         <v>.word 0x00000039</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>A40</v>
       </c>
       <c r="E84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2624</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <f t="shared" si="7"/>
+        <v>2.1145787545787544</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>58</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000003A</v>
       </c>
       <c r="C85" t="str">
@@ -2321,20 +2653,24 @@
         <v>.word 0x0000003A</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>A60</v>
       </c>
       <c r="E85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2656</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <f t="shared" si="7"/>
+        <v>2.1403663003663005</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>59</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000003B</v>
       </c>
       <c r="C86" t="str">
@@ -2342,20 +2678,24 @@
         <v>.word 0x0000003B</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>A80</v>
       </c>
       <c r="E86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2688</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <f t="shared" si="7"/>
+        <v>2.1661538461538461</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>60</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000003C</v>
       </c>
       <c r="C87" t="str">
@@ -2363,20 +2703,24 @@
         <v>.word 0x0000003C</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AA0</v>
       </c>
       <c r="E87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2720</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <f t="shared" si="7"/>
+        <v>2.1919413919413917</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>61</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000003D</v>
       </c>
       <c r="C88" t="str">
@@ -2384,20 +2728,24 @@
         <v>.word 0x0000003D</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AC0</v>
       </c>
       <c r="E88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2752</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <f t="shared" si="7"/>
+        <v>2.2177289377289378</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>62</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000003E</v>
       </c>
       <c r="C89" t="str">
@@ -2405,20 +2753,24 @@
         <v>.word 0x0000003E</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AE0</v>
       </c>
       <c r="E89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2784</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <f t="shared" si="7"/>
+        <v>2.2435164835164834</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>63</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000003F</v>
       </c>
       <c r="C90" t="str">
@@ -2426,20 +2778,24 @@
         <v>.word 0x0000003F</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>B00</v>
       </c>
       <c r="E90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2816</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <f t="shared" si="7"/>
+        <v>2.269304029304029</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>64</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000040</v>
       </c>
       <c r="C91" t="str">
@@ -2447,20 +2803,24 @@
         <v>.word 0x00000040</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>B20</v>
       </c>
       <c r="E91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2848</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <f t="shared" si="7"/>
+        <v>2.295091575091575</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>65</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000041</v>
       </c>
       <c r="C92" t="str">
@@ -2468,20 +2828,24 @@
         <v>.word 0x00000041</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>B40</v>
       </c>
       <c r="E92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2880</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <f t="shared" si="7"/>
+        <v>2.3208791208791211</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>66</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000042</v>
       </c>
       <c r="C93" t="str">
@@ -2489,20 +2853,24 @@
         <v>.word 0x00000042</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>B60</v>
       </c>
       <c r="E93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2912</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <f t="shared" si="7"/>
+        <v>2.3466666666666667</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>67</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000043</v>
       </c>
       <c r="C94" t="str">
@@ -2510,20 +2878,24 @@
         <v>.word 0x00000043</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>B80</v>
       </c>
       <c r="E94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2944</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <f t="shared" si="7"/>
+        <v>2.3724542124542123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>68</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000044</v>
       </c>
       <c r="C95" t="str">
@@ -2531,20 +2903,24 @@
         <v>.word 0x00000044</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>BA0</v>
       </c>
       <c r="E95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2976</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <f t="shared" si="7"/>
+        <v>2.3982417582417579</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>69</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000045</v>
       </c>
       <c r="C96" t="str">
@@ -2552,20 +2928,24 @@
         <v>.word 0x00000045</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>BC0</v>
       </c>
       <c r="E96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3008</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <f t="shared" si="7"/>
+        <v>2.4240293040293039</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>70</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000046</v>
       </c>
       <c r="C97" t="str">
@@ -2573,20 +2953,24 @@
         <v>.word 0x00000046</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>BE0</v>
       </c>
       <c r="E97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3040</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <f t="shared" si="7"/>
+        <v>2.44981684981685</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>71</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000047</v>
       </c>
       <c r="C98" t="str">
@@ -2594,20 +2978,24 @@
         <v>.word 0x00000047</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C00</v>
       </c>
       <c r="E98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3072</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <f t="shared" si="7"/>
+        <v>2.4756043956043956</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>72</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000048</v>
       </c>
       <c r="C99" t="str">
@@ -2615,20 +3003,24 @@
         <v>.word 0x00000048</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C20</v>
       </c>
       <c r="E99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3104</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <f t="shared" si="7"/>
+        <v>2.5013919413919412</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>73</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000049</v>
       </c>
       <c r="C100" t="str">
@@ -2636,20 +3028,24 @@
         <v>.word 0x00000049</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C40</v>
       </c>
       <c r="E100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3136</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <f t="shared" si="7"/>
+        <v>2.5271794871794873</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>74</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000004A</v>
       </c>
       <c r="C101" t="str">
@@ -2657,20 +3053,24 @@
         <v>.word 0x0000004A</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C60</v>
       </c>
       <c r="E101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3168</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <f t="shared" si="7"/>
+        <v>2.5529670329670329</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>75</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000004B</v>
       </c>
       <c r="C102" t="str">
@@ -2678,20 +3078,24 @@
         <v>.word 0x0000004B</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C80</v>
       </c>
       <c r="E102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3200</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <f t="shared" si="7"/>
+        <v>2.5787545787545785</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>76</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000004C</v>
       </c>
       <c r="C103" t="str">
@@ -2699,20 +3103,24 @@
         <v>.word 0x0000004C</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CA0</v>
       </c>
       <c r="E103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3232</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <f t="shared" si="7"/>
+        <v>2.6045421245421245</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>77</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000004D</v>
       </c>
       <c r="C104" t="str">
@@ -2720,20 +3128,24 @@
         <v>.word 0x0000004D</v>
       </c>
       <c r="D104" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CC0</v>
       </c>
       <c r="E104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3264</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <f t="shared" si="7"/>
+        <v>2.6303296703296706</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>78</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000004E</v>
       </c>
       <c r="C105" t="str">
@@ -2741,20 +3153,24 @@
         <v>.word 0x0000004E</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CE0</v>
       </c>
       <c r="E105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3296</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <f t="shared" si="7"/>
+        <v>2.6561172161172162</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>79</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000004F</v>
       </c>
       <c r="C106" t="str">
@@ -2762,20 +3178,24 @@
         <v>.word 0x0000004F</v>
       </c>
       <c r="D106" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>D00</v>
       </c>
       <c r="E106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3328</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <f t="shared" si="7"/>
+        <v>2.6819047619047618</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>80</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000050</v>
       </c>
       <c r="C107" t="str">
@@ -2783,20 +3203,24 @@
         <v>.word 0x00000050</v>
       </c>
       <c r="D107" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>D20</v>
       </c>
       <c r="E107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3360</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <f t="shared" si="7"/>
+        <v>2.7076923076923074</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>81</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000051</v>
       </c>
       <c r="C108" t="str">
@@ -2804,20 +3228,24 @@
         <v>.word 0x00000051</v>
       </c>
       <c r="D108" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>D40</v>
       </c>
       <c r="E108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3392</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <f t="shared" si="7"/>
+        <v>2.7334798534798534</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>82</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000052</v>
       </c>
       <c r="C109" t="str">
@@ -2825,20 +3253,24 @@
         <v>.word 0x00000052</v>
       </c>
       <c r="D109" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>D60</v>
       </c>
       <c r="E109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3424</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <f t="shared" si="7"/>
+        <v>2.7592673992673991</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>83</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000053</v>
       </c>
       <c r="C110" t="str">
@@ -2846,20 +3278,24 @@
         <v>.word 0x00000053</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>D80</v>
       </c>
       <c r="E110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3456</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110">
+        <f t="shared" si="7"/>
+        <v>2.7850549450549451</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>84</v>
       </c>
       <c r="B111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000054</v>
       </c>
       <c r="C111" t="str">
@@ -2867,20 +3303,24 @@
         <v>.word 0x00000054</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DA0</v>
       </c>
       <c r="E111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3488</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111">
+        <f t="shared" si="7"/>
+        <v>2.8108424908424907</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>85</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000055</v>
       </c>
       <c r="C112" t="str">
@@ -2888,20 +3328,24 @@
         <v>.word 0x00000055</v>
       </c>
       <c r="D112" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DC0</v>
       </c>
       <c r="E112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3520</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112">
+        <f t="shared" si="7"/>
+        <v>2.8366300366300368</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>86</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000056</v>
       </c>
       <c r="C113" t="str">
@@ -2909,20 +3353,24 @@
         <v>.word 0x00000056</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DE0</v>
       </c>
       <c r="E113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3552</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113">
+        <f t="shared" si="7"/>
+        <v>2.8624175824175824</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>87</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000057</v>
       </c>
       <c r="C114" t="str">
@@ -2930,20 +3378,24 @@
         <v>.word 0x00000057</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E00</v>
       </c>
       <c r="E114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3584</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114">
+        <f t="shared" si="7"/>
+        <v>2.888205128205128</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>88</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000058</v>
       </c>
       <c r="C115" t="str">
@@ -2951,20 +3403,24 @@
         <v>.word 0x00000058</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E20</v>
       </c>
       <c r="E115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3616</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115">
+        <f t="shared" si="7"/>
+        <v>2.9139926739926736</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>89</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000059</v>
       </c>
       <c r="C116" t="str">
@@ -2972,20 +3428,24 @@
         <v>.word 0x00000059</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E40</v>
       </c>
       <c r="E116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3648</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116">
+        <f t="shared" si="7"/>
+        <v>2.9397802197802196</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>90</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000005A</v>
       </c>
       <c r="C117" t="str">
@@ -2993,20 +3453,24 @@
         <v>.word 0x0000005A</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E60</v>
       </c>
       <c r="E117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3680</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117">
+        <f t="shared" si="7"/>
+        <v>2.9655677655677657</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>91</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000005B</v>
       </c>
       <c r="C118" t="str">
@@ -3014,20 +3478,24 @@
         <v>.word 0x0000005B</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>E80</v>
       </c>
       <c r="E118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3712</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118">
+        <f t="shared" si="7"/>
+        <v>2.9913553113553113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>92</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000005C</v>
       </c>
       <c r="C119" t="str">
@@ -3035,20 +3503,24 @@
         <v>.word 0x0000005C</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>EA0</v>
       </c>
       <c r="E119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3744</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119">
+        <f t="shared" si="7"/>
+        <v>3.0171428571428569</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>93</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000005D</v>
       </c>
       <c r="C120" t="str">
@@ -3056,20 +3528,24 @@
         <v>.word 0x0000005D</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>EC0</v>
       </c>
       <c r="E120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3776</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120">
+        <f t="shared" si="7"/>
+        <v>3.042930402930403</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>94</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000005E</v>
       </c>
       <c r="C121" t="str">
@@ -3077,20 +3553,24 @@
         <v>.word 0x0000005E</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>EE0</v>
       </c>
       <c r="E121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3808</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121">
+        <f t="shared" si="7"/>
+        <v>3.0687179487179486</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>95</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0000005F</v>
       </c>
       <c r="C122" t="str">
@@ -3098,20 +3578,24 @@
         <v>.word 0x0000005F</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>F00</v>
       </c>
       <c r="E122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3840</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122">
+        <f t="shared" si="7"/>
+        <v>3.0945054945054942</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>96</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000060</v>
       </c>
       <c r="C123" t="str">
@@ -3119,20 +3603,24 @@
         <v>.word 0x00000060</v>
       </c>
       <c r="D123" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>F20</v>
       </c>
       <c r="E123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3872</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123">
+        <f t="shared" si="7"/>
+        <v>3.1202930402930402</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>97</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000061</v>
       </c>
       <c r="C124" t="str">
@@ -3140,20 +3628,24 @@
         <v>.word 0x00000061</v>
       </c>
       <c r="D124" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>F40</v>
       </c>
       <c r="E124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3904</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124">
+        <f t="shared" si="7"/>
+        <v>3.1460805860805863</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>98</v>
       </c>
       <c r="B125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000062</v>
       </c>
       <c r="C125" t="str">
@@ -3161,20 +3653,24 @@
         <v>.word 0x00000062</v>
       </c>
       <c r="D125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>F60</v>
       </c>
       <c r="E125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3936</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125">
+        <f t="shared" si="7"/>
+        <v>3.1718681318681319</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>99</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000063</v>
       </c>
       <c r="C126" t="str">
@@ -3182,20 +3678,24 @@
         <v>.word 0x00000063</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>F80</v>
       </c>
       <c r="E126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3968</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126">
+        <f t="shared" si="7"/>
+        <v>3.1976556776556775</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>100</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000064</v>
       </c>
       <c r="C127" t="str">
@@ -3203,20 +3703,24 @@
         <v>.word 0x00000064</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>FA0</v>
       </c>
       <c r="E127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4000</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F127">
+        <f t="shared" si="7"/>
+        <v>3.2234432234432231</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>101</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000065</v>
       </c>
       <c r="C128" t="str">
@@ -3224,20 +3728,24 @@
         <v>.word 0x00000065</v>
       </c>
       <c r="D128" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>FC0</v>
       </c>
       <c r="E128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4032</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128">
+        <f t="shared" si="7"/>
+        <v>3.2492307692307691</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>102</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000066</v>
       </c>
       <c r="C129" t="str">
@@ -3245,20 +3753,24 @@
         <v>.word 0x00000066</v>
       </c>
       <c r="D129" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>FE0</v>
       </c>
       <c r="E129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4064</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129">
+        <f t="shared" si="7"/>
+        <v>3.2750183150183148</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>103</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000067</v>
       </c>
       <c r="C130" t="str">
@@ -3270,8 +3782,12 @@
         <v>FFF</v>
       </c>
       <c r="E130">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4095</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="7"/>
+        <v>3.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>